<commit_message>
Finished DataReader and DataUpdater. 'Aktualizuj zajetosc' button works. Started ResourceReader and ResourceUpdater.
</commit_message>
<xml_diff>
--- a/BusyForcast/240849.xlsx
+++ b/BusyForcast/240849.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wojciech.drozd\Desktop\prognoza_czasu_pracy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\BusyForcastRepo\BusyForcast\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2458,184 +2458,184 @@
                 <c:formatCode>#\ ##0.00_ ;[Red]\-#\ ##0.00\ </c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>-281719</c:v>
+                  <c:v>-709329.39999999991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-522295</c:v>
+                  <c:v>-1043489.7999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-762871</c:v>
+                  <c:v>-1463982.5999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1003447</c:v>
+                  <c:v>-1704558.5999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1244023</c:v>
+                  <c:v>-1974685.7999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1484599</c:v>
+                  <c:v>-2215261.7999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1725175</c:v>
+                  <c:v>-2455837.7999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1953351</c:v>
+                  <c:v>-2684013.7999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2193927</c:v>
+                  <c:v>-2924589.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2393723</c:v>
+                  <c:v>-3124385.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2634299</c:v>
+                  <c:v>-3364961.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-2860335</c:v>
+                  <c:v>-3590997.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2860335</c:v>
+                  <c:v>-3590997.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2864174.3220000002</c:v>
+                  <c:v>-3594837.122</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2864174.3220000002</c:v>
+                  <c:v>-3594837.122</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2882437.8140000002</c:v>
+                  <c:v>-3613100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2882437.8140000002</c:v>
+                  <c:v>-3613100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2882437.8140000002</c:v>
+                  <c:v>-3613100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2882437.8140000002</c:v>
+                  <c:v>-3613100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-2882437.8140000002</c:v>
+                  <c:v>-3613100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-2882437.8140000002</c:v>
+                  <c:v>-3613100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-2879437.8140000002</c:v>
+                  <c:v>-3610100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-2879437.8140000002</c:v>
+                  <c:v>-3610100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-2879437.8140000002</c:v>
+                  <c:v>-3610100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-2879437.8140000002</c:v>
+                  <c:v>-3610100.6140000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-2888589.0960000004</c:v>
+                  <c:v>-3619251.8960000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4820,22 +4820,22 @@
       </c>
       <c r="C15" s="179">
         <f>SUM(D15:BL15)</f>
-        <v>1081380.3199999998</v>
+        <v>1342331.3199999998</v>
       </c>
       <c r="D15" s="146">
         <v>43896</v>
       </c>
       <c r="E15" s="127">
         <f>Days!F222</f>
-        <v>85920</v>
+        <v>238638</v>
       </c>
       <c r="F15" s="127">
         <f>Days!G222</f>
-        <v>85920</v>
+        <v>119343</v>
       </c>
       <c r="G15" s="127">
         <f>Days!H222</f>
-        <v>85920</v>
+        <v>150176</v>
       </c>
       <c r="H15" s="127">
         <f>Days!I222</f>
@@ -4843,7 +4843,7 @@
       </c>
       <c r="I15" s="127">
         <f>Days!J222</f>
-        <v>85920</v>
+        <v>96474</v>
       </c>
       <c r="J15" s="127">
         <f>Days!K222</f>
@@ -5073,20 +5073,20 @@
       </c>
       <c r="C16" s="119">
         <f>SUM(E16:BM16)</f>
-        <v>1867471.7759999998</v>
+        <v>2337183.5759999999</v>
       </c>
       <c r="D16" s="146"/>
       <c r="E16" s="127">
         <f>Days!F223</f>
-        <v>154656</v>
+        <v>429548.39999999997</v>
       </c>
       <c r="F16" s="127">
         <f>Days!G223</f>
-        <v>154656</v>
+        <v>214817.4</v>
       </c>
       <c r="G16" s="127">
         <f>Days!H223</f>
-        <v>154656</v>
+        <v>270316.79999999999</v>
       </c>
       <c r="H16" s="127">
         <f>Days!I223</f>
@@ -5094,7 +5094,7 @@
       </c>
       <c r="I16" s="127">
         <f>Days!J223</f>
-        <v>154656</v>
+        <v>173653.2</v>
       </c>
       <c r="J16" s="127">
         <f>Days!K223</f>
@@ -5738,22 +5738,22 @@
       </c>
       <c r="C18" s="119">
         <f>C16+C17+D18</f>
-        <v>1946565.7759999998</v>
+        <v>2416277.5759999999</v>
       </c>
       <c r="D18" s="146">
         <v>79094</v>
       </c>
       <c r="E18" s="127">
         <f t="shared" ref="E18:AJ18" si="4">E17+E16</f>
-        <v>154656</v>
+        <v>429548.39999999997</v>
       </c>
       <c r="F18" s="58">
         <f t="shared" si="4"/>
-        <v>154656</v>
+        <v>214817.4</v>
       </c>
       <c r="G18" s="58">
         <f t="shared" si="4"/>
-        <v>154656</v>
+        <v>270316.79999999999</v>
       </c>
       <c r="H18" s="58">
         <f t="shared" si="4"/>
@@ -5761,7 +5761,7 @@
       </c>
       <c r="I18" s="58">
         <f t="shared" si="4"/>
-        <v>154656</v>
+        <v>173653.2</v>
       </c>
       <c r="J18" s="58">
         <f t="shared" si="4"/>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="C19" s="119">
         <f>C15+C18</f>
-        <v>3027946.0959999999</v>
+        <v>3758608.8959999997</v>
       </c>
       <c r="D19" s="161">
         <f t="shared" ref="D19:BL19" si="6">D15+D18</f>
@@ -6162,15 +6162,15 @@
       </c>
       <c r="E19" s="161">
         <f t="shared" si="6"/>
-        <v>240576</v>
+        <v>668186.39999999991</v>
       </c>
       <c r="F19" s="161">
         <f t="shared" si="6"/>
-        <v>240576</v>
+        <v>334160.40000000002</v>
       </c>
       <c r="G19" s="161">
         <f t="shared" si="6"/>
-        <v>240576</v>
+        <v>420492.79999999999</v>
       </c>
       <c r="H19" s="161">
         <f t="shared" si="6"/>
@@ -6178,7 +6178,7 @@
       </c>
       <c r="I19" s="161">
         <f t="shared" si="6"/>
-        <v>240576</v>
+        <v>270127.2</v>
       </c>
       <c r="J19" s="161">
         <f t="shared" si="6"/>
@@ -6571,7 +6571,7 @@
       </c>
       <c r="C20" s="132">
         <f>C18/C15</f>
-        <v>1.8000750892156057</v>
+        <v>1.8000604917718825</v>
       </c>
       <c r="D20" s="132">
         <f>D18/D15</f>
@@ -7247,7 +7247,7 @@
       </c>
       <c r="C24" s="118">
         <f>C23+C19</f>
-        <v>3044499.0959999999</v>
+        <v>3775161.8959999997</v>
       </c>
       <c r="D24" s="162">
         <f t="shared" ref="D24:BL24" si="9">D23+D19</f>
@@ -7255,15 +7255,15 @@
       </c>
       <c r="E24" s="162">
         <f t="shared" si="9"/>
-        <v>240576</v>
+        <v>668186.39999999991</v>
       </c>
       <c r="F24" s="162">
         <f t="shared" si="9"/>
-        <v>240576</v>
+        <v>334160.40000000002</v>
       </c>
       <c r="G24" s="162">
         <f t="shared" si="9"/>
-        <v>240576</v>
+        <v>420492.79999999999</v>
       </c>
       <c r="H24" s="162">
         <f t="shared" si="9"/>
@@ -7271,7 +7271,7 @@
       </c>
       <c r="I24" s="162">
         <f t="shared" si="9"/>
-        <v>240576</v>
+        <v>270127.2</v>
       </c>
       <c r="J24" s="162">
         <f t="shared" si="9"/>
@@ -7503,243 +7503,243 @@
       <c r="D25" s="174"/>
       <c r="E25" s="175">
         <f>D24+E24</f>
-        <v>366219</v>
+        <v>793829.39999999991</v>
       </c>
       <c r="F25" s="176">
         <f>E25+F24</f>
-        <v>606795</v>
+        <v>1127989.7999999998</v>
       </c>
       <c r="G25" s="176">
         <f t="shared" ref="G25:BK25" si="10">F25+G24</f>
-        <v>847371</v>
+        <v>1548482.5999999999</v>
       </c>
       <c r="H25" s="176">
         <f t="shared" si="10"/>
-        <v>1087947</v>
+        <v>1789058.5999999999</v>
       </c>
       <c r="I25" s="176">
         <f t="shared" si="10"/>
-        <v>1328523</v>
+        <v>2059185.7999999998</v>
       </c>
       <c r="J25" s="176">
         <f t="shared" si="10"/>
-        <v>1569099</v>
+        <v>2299761.7999999998</v>
       </c>
       <c r="K25" s="176">
         <f t="shared" si="10"/>
-        <v>1809675</v>
+        <v>2540337.7999999998</v>
       </c>
       <c r="L25" s="176">
         <f t="shared" si="10"/>
-        <v>2050251</v>
+        <v>2780913.8</v>
       </c>
       <c r="M25" s="176">
         <f t="shared" si="10"/>
-        <v>2290827</v>
+        <v>3021489.8</v>
       </c>
       <c r="N25" s="176">
         <f t="shared" si="10"/>
-        <v>2531403</v>
+        <v>3262065.8</v>
       </c>
       <c r="O25" s="176">
         <f t="shared" si="10"/>
-        <v>2771979</v>
+        <v>3502641.8</v>
       </c>
       <c r="P25" s="176">
         <f t="shared" si="10"/>
-        <v>3012555</v>
+        <v>3743217.8</v>
       </c>
       <c r="Q25" s="176">
         <f t="shared" si="10"/>
-        <v>3012555</v>
+        <v>3743217.8</v>
       </c>
       <c r="R25" s="176">
         <f t="shared" si="10"/>
-        <v>3017084.3220000002</v>
+        <v>3747747.122</v>
       </c>
       <c r="S25" s="176">
         <f t="shared" si="10"/>
-        <v>3017084.3220000002</v>
+        <v>3747747.122</v>
       </c>
       <c r="T25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="U25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="V25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="W25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="X25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="Y25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="Z25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="AA25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="AB25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="AC25" s="176">
         <f t="shared" si="10"/>
-        <v>3035347.8140000002</v>
+        <v>3766010.6140000001</v>
       </c>
       <c r="AD25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AE25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AF25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AG25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AH25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AI25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AJ25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AK25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AL25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AM25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AN25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AO25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AP25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AQ25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AR25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AS25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AT25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AU25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AV25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AW25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AX25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AY25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="AZ25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BA25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BB25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BC25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BD25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BE25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BF25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BG25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BH25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BI25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BJ25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BK25" s="176">
         <f t="shared" si="10"/>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
       <c r="BL25" s="177">
         <f>BK25+BL24</f>
-        <v>3044499.0960000004</v>
+        <v>3775161.8960000002</v>
       </c>
     </row>
     <row r="26" spans="1:227" s="124" customFormat="1" x14ac:dyDescent="0.2">
@@ -7749,7 +7749,7 @@
       </c>
       <c r="C26" s="121">
         <f>C9-C24</f>
-        <v>-2815199.0959999999</v>
+        <v>-3545861.8959999997</v>
       </c>
       <c r="D26" s="148">
         <f>D9-D24</f>
@@ -7757,243 +7757,243 @@
       </c>
       <c r="E26" s="137">
         <f t="shared" ref="E26:AJ26" si="11">E13-E25</f>
-        <v>-208329</v>
+        <v>-635939.39999999991</v>
       </c>
       <c r="F26" s="122">
         <f t="shared" si="11"/>
-        <v>-448905</v>
+        <v>-970099.79999999981</v>
       </c>
       <c r="G26" s="122">
         <f t="shared" si="11"/>
-        <v>-689481</v>
+        <v>-1390592.5999999999</v>
       </c>
       <c r="H26" s="122">
         <f t="shared" si="11"/>
-        <v>-930057</v>
+        <v>-1631168.5999999999</v>
       </c>
       <c r="I26" s="122">
         <f t="shared" si="11"/>
-        <v>-1170633</v>
+        <v>-1901295.7999999998</v>
       </c>
       <c r="J26" s="122">
         <f t="shared" si="11"/>
-        <v>-1398809</v>
+        <v>-2129471.7999999998</v>
       </c>
       <c r="K26" s="122">
         <f t="shared" si="11"/>
-        <v>-1639385</v>
+        <v>-2370047.7999999998</v>
       </c>
       <c r="L26" s="122">
         <f t="shared" si="11"/>
-        <v>-1839181</v>
+        <v>-2569843.7999999998</v>
       </c>
       <c r="M26" s="122">
         <f t="shared" si="11"/>
-        <v>-2079757</v>
+        <v>-2810419.8</v>
       </c>
       <c r="N26" s="122">
         <f t="shared" si="11"/>
-        <v>-2305793</v>
+        <v>-3036455.8</v>
       </c>
       <c r="O26" s="122">
         <f t="shared" si="11"/>
-        <v>-2546369</v>
+        <v>-3277031.8</v>
       </c>
       <c r="P26" s="122">
         <f t="shared" si="11"/>
-        <v>-2786255</v>
+        <v>-3516917.8</v>
       </c>
       <c r="Q26" s="122">
         <f t="shared" si="11"/>
-        <v>-2786255</v>
+        <v>-3516917.8</v>
       </c>
       <c r="R26" s="122">
         <f t="shared" si="11"/>
-        <v>-2790784.3220000002</v>
+        <v>-3521447.122</v>
       </c>
       <c r="S26" s="122">
         <f t="shared" si="11"/>
-        <v>-2790784.3220000002</v>
+        <v>-3521447.122</v>
       </c>
       <c r="T26" s="122">
         <f t="shared" si="11"/>
-        <v>-2809047.8140000002</v>
+        <v>-3539710.6140000001</v>
       </c>
       <c r="U26" s="122">
         <f t="shared" si="11"/>
-        <v>-2809047.8140000002</v>
+        <v>-3539710.6140000001</v>
       </c>
       <c r="V26" s="122">
         <f t="shared" si="11"/>
-        <v>-2809047.8140000002</v>
+        <v>-3539710.6140000001</v>
       </c>
       <c r="W26" s="122">
         <f t="shared" si="11"/>
-        <v>-2809047.8140000002</v>
+        <v>-3539710.6140000001</v>
       </c>
       <c r="X26" s="122">
         <f t="shared" si="11"/>
-        <v>-2806047.8140000002</v>
+        <v>-3536710.6140000001</v>
       </c>
       <c r="Y26" s="122">
         <f t="shared" si="11"/>
-        <v>-2806047.8140000002</v>
+        <v>-3536710.6140000001</v>
       </c>
       <c r="Z26" s="122">
         <f t="shared" si="11"/>
-        <v>-2806047.8140000002</v>
+        <v>-3536710.6140000001</v>
       </c>
       <c r="AA26" s="122">
         <f t="shared" si="11"/>
-        <v>-2806047.8140000002</v>
+        <v>-3536710.6140000001</v>
       </c>
       <c r="AB26" s="122">
         <f t="shared" si="11"/>
-        <v>-2806047.8140000002</v>
+        <v>-3536710.6140000001</v>
       </c>
       <c r="AC26" s="122">
         <f t="shared" si="11"/>
-        <v>-2806047.8140000002</v>
+        <v>-3536710.6140000001</v>
       </c>
       <c r="AD26" s="122">
         <f t="shared" si="11"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AE26" s="122">
         <f t="shared" si="11"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AF26" s="122">
         <f t="shared" si="11"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AG26" s="122">
         <f t="shared" si="11"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AH26" s="122">
         <f t="shared" si="11"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AI26" s="122">
         <f t="shared" si="11"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AJ26" s="122">
         <f t="shared" si="11"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AK26" s="122">
         <f t="shared" ref="AK26:BL26" si="12">AK13-AK25</f>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AL26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AM26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AN26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AO26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AP26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AQ26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AR26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AS26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AT26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AU26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AV26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AW26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AX26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AY26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="AZ26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BA26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BB26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BC26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BD26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BE26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BF26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BG26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BH26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BI26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BJ26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BK26" s="122">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
       <c r="BL26" s="123">
         <f t="shared" si="12"/>
-        <v>-2815199.0960000004</v>
+        <v>-3545861.8960000002</v>
       </c>
     </row>
     <row r="27" spans="1:227" s="45" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="C27" s="155">
         <f>C26/C9</f>
-        <v>-12.277361953772351</v>
+        <v>-15.463854757959004</v>
       </c>
       <c r="D27" s="149">
         <f>D26/D9</f>
@@ -8082,243 +8082,243 @@
       </c>
       <c r="E28" s="139">
         <f>E14-E25</f>
-        <v>-281719</v>
+        <v>-709329.39999999991</v>
       </c>
       <c r="F28" s="39">
         <f t="shared" ref="F28:AJ28" si="13">F14-F25</f>
-        <v>-522295</v>
+        <v>-1043489.7999999998</v>
       </c>
       <c r="G28" s="39">
         <f t="shared" si="13"/>
-        <v>-762871</v>
+        <v>-1463982.5999999999</v>
       </c>
       <c r="H28" s="39">
         <f t="shared" si="13"/>
-        <v>-1003447</v>
+        <v>-1704558.5999999999</v>
       </c>
       <c r="I28" s="39">
         <f t="shared" si="13"/>
-        <v>-1244023</v>
+        <v>-1974685.7999999998</v>
       </c>
       <c r="J28" s="39">
         <f t="shared" si="13"/>
-        <v>-1484599</v>
+        <v>-2215261.7999999998</v>
       </c>
       <c r="K28" s="39">
         <f t="shared" si="13"/>
-        <v>-1725175</v>
+        <v>-2455837.7999999998</v>
       </c>
       <c r="L28" s="39">
         <f t="shared" si="13"/>
-        <v>-1953351</v>
+        <v>-2684013.7999999998</v>
       </c>
       <c r="M28" s="39">
         <f t="shared" si="13"/>
-        <v>-2193927</v>
+        <v>-2924589.8</v>
       </c>
       <c r="N28" s="39">
         <f t="shared" si="13"/>
-        <v>-2393723</v>
+        <v>-3124385.8</v>
       </c>
       <c r="O28" s="39">
         <f t="shared" si="13"/>
-        <v>-2634299</v>
+        <v>-3364961.8</v>
       </c>
       <c r="P28" s="39">
         <f t="shared" si="13"/>
-        <v>-2860335</v>
+        <v>-3590997.8</v>
       </c>
       <c r="Q28" s="39">
         <f t="shared" si="13"/>
-        <v>-2860335</v>
+        <v>-3590997.8</v>
       </c>
       <c r="R28" s="39">
         <f t="shared" si="13"/>
-        <v>-2864174.3220000002</v>
+        <v>-3594837.122</v>
       </c>
       <c r="S28" s="39">
         <f t="shared" si="13"/>
-        <v>-2864174.3220000002</v>
+        <v>-3594837.122</v>
       </c>
       <c r="T28" s="39">
         <f t="shared" si="13"/>
-        <v>-2882437.8140000002</v>
+        <v>-3613100.6140000001</v>
       </c>
       <c r="U28" s="39">
         <f t="shared" si="13"/>
-        <v>-2882437.8140000002</v>
+        <v>-3613100.6140000001</v>
       </c>
       <c r="V28" s="39">
         <f t="shared" si="13"/>
-        <v>-2882437.8140000002</v>
+        <v>-3613100.6140000001</v>
       </c>
       <c r="W28" s="39">
         <f t="shared" si="13"/>
-        <v>-2882437.8140000002</v>
+        <v>-3613100.6140000001</v>
       </c>
       <c r="X28" s="39">
         <f t="shared" si="13"/>
-        <v>-2882437.8140000002</v>
+        <v>-3613100.6140000001</v>
       </c>
       <c r="Y28" s="39">
         <f t="shared" si="13"/>
-        <v>-2882437.8140000002</v>
+        <v>-3613100.6140000001</v>
       </c>
       <c r="Z28" s="39">
         <f t="shared" si="13"/>
-        <v>-2879437.8140000002</v>
+        <v>-3610100.6140000001</v>
       </c>
       <c r="AA28" s="39">
         <f t="shared" si="13"/>
-        <v>-2879437.8140000002</v>
+        <v>-3610100.6140000001</v>
       </c>
       <c r="AB28" s="39">
         <f t="shared" si="13"/>
-        <v>-2879437.8140000002</v>
+        <v>-3610100.6140000001</v>
       </c>
       <c r="AC28" s="39">
         <f t="shared" si="13"/>
-        <v>-2879437.8140000002</v>
+        <v>-3610100.6140000001</v>
       </c>
       <c r="AD28" s="39">
         <f t="shared" si="13"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AE28" s="39">
         <f t="shared" si="13"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AF28" s="39">
         <f t="shared" si="13"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AG28" s="39">
         <f t="shared" si="13"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AH28" s="39">
         <f t="shared" si="13"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AI28" s="39">
         <f t="shared" si="13"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AJ28" s="39">
         <f t="shared" si="13"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AK28" s="39">
         <f t="shared" ref="AK28:BL28" si="14">AK14-AK25</f>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AL28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AM28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AN28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AO28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AP28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AQ28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AR28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AS28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AT28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AU28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AV28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AW28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AX28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AY28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="AZ28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BA28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BB28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BC28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BD28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BE28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BF28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BG28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BH28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BI28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BJ28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BK28" s="39">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
       <c r="BL28" s="40">
         <f t="shared" si="14"/>
-        <v>-2888589.0960000004</v>
+        <v>-3619251.8960000002</v>
       </c>
     </row>
     <row r="29" spans="1:227" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -8327,7 +8327,7 @@
       </c>
       <c r="C29" s="237">
         <f>(C26+C22)/C9</f>
-        <v>-12.216742677714784</v>
+        <v>-15.403235481901438</v>
       </c>
     </row>
     <row r="32" spans="1:227" x14ac:dyDescent="0.2">
@@ -9034,8 +9034,8 @@
   <dimension ref="A1:BM230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+      <pane ySplit="10" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F214" sqref="F214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22706,9 +22706,11 @@
       <c r="D99" s="89"/>
       <c r="E99" s="227">
         <f>SUM(F99:BM99)</f>
-        <v>0</v>
-      </c>
-      <c r="F99" s="70"/>
+        <v>6</v>
+      </c>
+      <c r="F99" s="70">
+        <v>6</v>
+      </c>
       <c r="G99" s="70"/>
       <c r="H99" s="70"/>
       <c r="I99" s="70"/>
@@ -22928,9 +22930,11 @@
       <c r="D102" s="89"/>
       <c r="E102" s="227">
         <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="F102" s="70"/>
+        <v>6</v>
+      </c>
+      <c r="F102" s="70">
+        <v>6</v>
+      </c>
       <c r="G102" s="70"/>
       <c r="H102" s="70"/>
       <c r="I102" s="203"/>
@@ -23224,9 +23228,11 @@
       <c r="D106" s="89"/>
       <c r="E106" s="227">
         <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="F106" s="70"/>
+        <v>6</v>
+      </c>
+      <c r="F106" s="70">
+        <v>6</v>
+      </c>
       <c r="G106" s="70"/>
       <c r="H106" s="70"/>
       <c r="I106" s="70"/>
@@ -23298,9 +23304,11 @@
       <c r="D107" s="4"/>
       <c r="E107" s="227">
         <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="F107" s="70"/>
+        <v>6</v>
+      </c>
+      <c r="F107" s="70">
+        <v>6</v>
+      </c>
       <c r="G107" s="70"/>
       <c r="H107" s="70"/>
       <c r="I107" s="70"/>
@@ -23369,12 +23377,12 @@
       <c r="C108" s="17"/>
       <c r="D108" s="184">
         <f>SUM(F108:BM108)</f>
-        <v>0</v>
+        <v>20496</v>
       </c>
       <c r="E108" s="229"/>
       <c r="F108" s="13">
         <f>$C99*(1+F$7)*F99+$C100*(1+F$7)*F100+$C101*(1+F$7)*F101+$C102*(1+F$7)*F102+$C103*(1+F$7)*F103+$C104*(1+F$7)*F104+$C105*(1+F$7)*F105+$C106*(1+F$7)*F106+$C107*(1+F$7)*F107</f>
-        <v>0</v>
+        <v>20496</v>
       </c>
       <c r="G108" s="13">
         <f t="shared" ref="G108:BL108" si="69">$C99*(1+G$7)*G99+$C100*(1+G$7)*G100+$C101*(1+G$7)*G101+$C102*(1+G$7)*G102+$C103*(1+G$7)*G103+$C104*(1+G$7)*G104+$C105*(1+G$7)*G105+$C106*(1+G$7)*G106+$C107*(1+G$7)*G107</f>
@@ -23623,12 +23631,12 @@
       </c>
       <c r="D109" s="184">
         <f>SUM(F109:BM109)</f>
-        <v>0</v>
+        <v>36892.800000000003</v>
       </c>
       <c r="E109" s="229"/>
       <c r="F109" s="13">
         <f>$C109*F108</f>
-        <v>0</v>
+        <v>36892.800000000003</v>
       </c>
       <c r="G109" s="13">
         <f t="shared" ref="G109:BM109" si="70">$C109*G108</f>
@@ -24129,12 +24137,12 @@
       <c r="C111" s="90"/>
       <c r="D111" s="184">
         <f>SUM(F111:BM111)</f>
-        <v>0</v>
+        <v>57388.800000000003</v>
       </c>
       <c r="E111" s="230"/>
       <c r="F111" s="81">
         <f>F108+F109+F110</f>
-        <v>0</v>
+        <v>57388.800000000003</v>
       </c>
       <c r="G111" s="81">
         <f>G108+G109+G110</f>
@@ -24646,9 +24654,11 @@
       <c r="D114" s="201"/>
       <c r="E114" s="203">
         <f>SUM(F114:BM114)</f>
-        <v>0</v>
-      </c>
-      <c r="F114" s="203"/>
+        <v>7</v>
+      </c>
+      <c r="F114" s="203">
+        <v>7</v>
+      </c>
       <c r="G114" s="203"/>
       <c r="H114" s="203"/>
       <c r="I114" s="203"/>
@@ -24868,10 +24878,12 @@
       <c r="D117" s="201"/>
       <c r="E117" s="203">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F117" s="203"/>
-      <c r="G117" s="203"/>
+      <c r="G117" s="203">
+        <v>7</v>
+      </c>
       <c r="H117" s="203"/>
       <c r="I117" s="203"/>
       <c r="J117" s="203"/>
@@ -25164,11 +25176,13 @@
       <c r="D121" s="201"/>
       <c r="E121" s="203">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F121" s="203"/>
       <c r="G121" s="203"/>
-      <c r="H121" s="203"/>
+      <c r="H121" s="203">
+        <v>7</v>
+      </c>
       <c r="I121" s="203"/>
       <c r="J121" s="203"/>
       <c r="K121" s="203"/>
@@ -25238,9 +25252,11 @@
       <c r="D122" s="201"/>
       <c r="E122" s="203">
         <f t="shared" si="73"/>
-        <v>0</v>
-      </c>
-      <c r="F122" s="203"/>
+        <v>7</v>
+      </c>
+      <c r="F122" s="203">
+        <v>7</v>
+      </c>
       <c r="G122" s="203"/>
       <c r="H122" s="203"/>
       <c r="I122" s="203"/>
@@ -25309,20 +25325,20 @@
       <c r="C123" s="17"/>
       <c r="D123" s="184">
         <f>SUM(F123:BM123)</f>
-        <v>0</v>
+        <v>23912</v>
       </c>
       <c r="E123" s="229"/>
       <c r="F123" s="13">
         <f>$C114*(1+F$7)*F114+$C115*(1+F$7)*F115+$C116*(1+F$7)*F116+$C117*(1+F$7)*F117+$C118*(1+F$7)*F118+$C119*(1+F$7)*F119+$C120*(1+F$7)*F120+$C121*(1+F$7)*F121+$C122*(1+F$7)*F122</f>
-        <v>0</v>
+        <v>12908</v>
       </c>
       <c r="G123" s="13">
         <f>$C114*(1+G$7)*G114+$C115*(1+G$7)*G115+$C116*(1+G$7)*G116+$C117*(1+G$7)*G117+$C118*(1+G$7)*G118+$C119*(1+G$7)*G119+$C120*(1+G$7)*G120+$C121*(1+G$7)*G121+$C122*(1+G$7)*G122</f>
-        <v>0</v>
+        <v>2226</v>
       </c>
       <c r="H123" s="13">
         <f t="shared" ref="H123:BL123" si="74">$C114*(1+H$7)*H114+$C115*(1+H$7)*H115+$C116*(1+H$7)*H116+$C117*(1+H$7)*H117+$C118*(1+H$7)*H118+$C119*(1+H$7)*H119+$C120*(1+H$7)*H120+$C121*(1+H$7)*H121+$C122*(1+H$7)*H122</f>
-        <v>0</v>
+        <v>8778</v>
       </c>
       <c r="I123" s="13">
         <f t="shared" si="74"/>
@@ -25563,20 +25579,20 @@
       </c>
       <c r="D124" s="184">
         <f>SUM(F124:BM124)</f>
-        <v>0</v>
+        <v>43041.599999999999</v>
       </c>
       <c r="E124" s="229"/>
       <c r="F124" s="13">
         <f>$C124*F123</f>
-        <v>0</v>
+        <v>23234.400000000001</v>
       </c>
       <c r="G124" s="13">
         <f t="shared" ref="G124:BM124" si="75">$C124*G123</f>
-        <v>0</v>
+        <v>4006.8</v>
       </c>
       <c r="H124" s="13">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>15800.4</v>
       </c>
       <c r="I124" s="13">
         <f t="shared" si="75"/>
@@ -26069,23 +26085,23 @@
       <c r="C126" s="90"/>
       <c r="D126" s="184">
         <f>SUM(F126:BM126)</f>
-        <v>0</v>
+        <v>66953.600000000006</v>
       </c>
       <c r="E126" s="230">
         <f>+E116+E117+E120</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F126" s="81">
         <f>F123+F124+F125</f>
-        <v>0</v>
+        <v>36142.400000000001</v>
       </c>
       <c r="G126" s="81">
         <f>G123+G124+G125</f>
-        <v>0</v>
+        <v>6232.8</v>
       </c>
       <c r="H126" s="81">
         <f t="shared" ref="H126:BM126" si="77">H123+H124+H125</f>
-        <v>0</v>
+        <v>24578.400000000001</v>
       </c>
       <c r="I126" s="81">
         <f t="shared" si="77"/>
@@ -26589,9 +26605,11 @@
       <c r="D129" s="201"/>
       <c r="E129" s="203">
         <f>SUM(F129:BM129)</f>
-        <v>0</v>
-      </c>
-      <c r="F129" s="203"/>
+        <v>8</v>
+      </c>
+      <c r="F129" s="203">
+        <v>8</v>
+      </c>
       <c r="G129" s="203"/>
       <c r="H129" s="203"/>
       <c r="I129" s="203"/>
@@ -26737,9 +26755,11 @@
       <c r="D131" s="201"/>
       <c r="E131" s="203">
         <f t="shared" si="78"/>
-        <v>0</v>
-      </c>
-      <c r="F131" s="203"/>
+        <v>8</v>
+      </c>
+      <c r="F131" s="203">
+        <v>8</v>
+      </c>
       <c r="G131" s="203"/>
       <c r="H131" s="203"/>
       <c r="I131" s="203"/>
@@ -27033,10 +27053,12 @@
       <c r="D135" s="202"/>
       <c r="E135" s="203">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F135" s="203"/>
-      <c r="G135" s="203"/>
+      <c r="G135" s="203">
+        <v>8</v>
+      </c>
       <c r="H135" s="203"/>
       <c r="I135" s="203"/>
       <c r="J135" s="203"/>
@@ -27181,11 +27203,15 @@
       <c r="D137" s="201"/>
       <c r="E137" s="203">
         <f t="shared" si="78"/>
-        <v>0</v>
-      </c>
-      <c r="F137" s="203"/>
+        <v>16</v>
+      </c>
+      <c r="F137" s="203">
+        <v>8</v>
+      </c>
       <c r="G137" s="203"/>
-      <c r="H137" s="203"/>
+      <c r="H137" s="203">
+        <v>8</v>
+      </c>
       <c r="I137" s="203"/>
       <c r="J137" s="203"/>
       <c r="K137" s="203"/>
@@ -27252,20 +27278,20 @@
       <c r="C138" s="17"/>
       <c r="D138" s="184">
         <f>SUM(F138:BM138)</f>
-        <v>0</v>
+        <v>37704</v>
       </c>
       <c r="E138" s="229"/>
       <c r="F138" s="13">
         <f>$C129*(1+F$7)*F129+$C130*(1+F$7)*F130+$C131*(1+F$7)*F131+$C132*(1+F$7)*F132+$C133*(1+F$7)*F133+$C134*(1+F$7)*F134+$C135*(1+F$7)*F135+$C136*(1+F$7)*F136+$C137*(1+F$7)*F137</f>
-        <v>0</v>
+        <v>16608</v>
       </c>
       <c r="G138" s="13">
         <f>$C129*(1+G$7)*G129+$C130*(1+G$7)*G130+$C131*(1+G$7)*G131+$C132*(1+G$7)*G132+$C133*(1+G$7)*G133+$C134*(1+G$7)*G134+$C135*(1+G$7)*G135+$C136*(1+G$7)*G136+$C137*(1+G$7)*G137</f>
-        <v>0</v>
+        <v>7320</v>
       </c>
       <c r="H138" s="13">
         <f t="shared" ref="H138:BL138" si="79">$C129*(1+H$7)*H129+$C130*(1+H$7)*H130+$C131*(1+H$7)*H131+$C132*(1+H$7)*H132+$C133*(1+H$7)*H133+$C134*(1+H$7)*H134+$C135*(1+H$7)*H135+$C136*(1+H$7)*H136+$C137*(1+H$7)*H137</f>
-        <v>0</v>
+        <v>13776</v>
       </c>
       <c r="I138" s="13">
         <f t="shared" si="79"/>
@@ -27506,20 +27532,20 @@
       </c>
       <c r="D139" s="184">
         <f>SUM(F139:BM139)</f>
-        <v>0</v>
+        <v>67867.199999999997</v>
       </c>
       <c r="E139" s="229"/>
       <c r="F139" s="13">
         <f>$C139*F138</f>
-        <v>0</v>
+        <v>29894.400000000001</v>
       </c>
       <c r="G139" s="13">
         <f t="shared" ref="G139:BM139" si="80">$C139*G138</f>
-        <v>0</v>
+        <v>13176</v>
       </c>
       <c r="H139" s="13">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>24796.799999999999</v>
       </c>
       <c r="I139" s="13">
         <f t="shared" si="80"/>
@@ -28012,23 +28038,23 @@
       <c r="C141" s="90"/>
       <c r="D141" s="184">
         <f>SUM(F141:BM141)</f>
-        <v>0</v>
+        <v>105571.2</v>
       </c>
       <c r="E141" s="230">
         <f>+E131+E132+E135</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F141" s="81">
         <f>F138+F139+F140</f>
-        <v>0</v>
+        <v>46502.400000000001</v>
       </c>
       <c r="G141" s="81">
         <f>G138+G139+G140</f>
-        <v>0</v>
+        <v>20496</v>
       </c>
       <c r="H141" s="81">
         <f t="shared" ref="H141:BM141" si="82">H138+H139+H140</f>
-        <v>0</v>
+        <v>38572.800000000003</v>
       </c>
       <c r="I141" s="81">
         <f t="shared" si="82"/>
@@ -28532,9 +28558,11 @@
       <c r="D144" s="201"/>
       <c r="E144" s="203">
         <f>SUM(F144:BM144)</f>
-        <v>0</v>
-      </c>
-      <c r="F144" s="203"/>
+        <v>9</v>
+      </c>
+      <c r="F144" s="203">
+        <v>9</v>
+      </c>
       <c r="G144" s="203"/>
       <c r="H144" s="203"/>
       <c r="I144" s="203"/>
@@ -28754,9 +28782,11 @@
       <c r="D147" s="201"/>
       <c r="E147" s="203">
         <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="F147" s="203"/>
+        <v>9</v>
+      </c>
+      <c r="F147" s="203">
+        <v>9</v>
+      </c>
       <c r="G147" s="203"/>
       <c r="H147" s="203"/>
       <c r="I147" s="203"/>
@@ -28976,10 +29006,12 @@
       <c r="D150" s="202"/>
       <c r="E150" s="203">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F150" s="203"/>
-      <c r="G150" s="203"/>
+      <c r="G150" s="203">
+        <v>9</v>
+      </c>
       <c r="H150" s="203"/>
       <c r="I150" s="203"/>
       <c r="J150" s="203"/>
@@ -29050,11 +29082,15 @@
       <c r="D151" s="201"/>
       <c r="E151" s="203">
         <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="F151" s="203"/>
+        <v>18</v>
+      </c>
+      <c r="F151" s="203">
+        <v>9</v>
+      </c>
       <c r="G151" s="203"/>
-      <c r="H151" s="203"/>
+      <c r="H151" s="203">
+        <v>9</v>
+      </c>
       <c r="I151" s="203"/>
       <c r="J151" s="203"/>
       <c r="K151" s="203"/>
@@ -29124,9 +29160,11 @@
       <c r="D152" s="201"/>
       <c r="E152" s="203">
         <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="F152" s="203"/>
+        <v>9</v>
+      </c>
+      <c r="F152" s="203">
+        <v>9</v>
+      </c>
       <c r="G152" s="203"/>
       <c r="H152" s="203"/>
       <c r="I152" s="203"/>
@@ -29195,20 +29233,20 @@
       <c r="C153" s="17"/>
       <c r="D153" s="184">
         <f>SUM(F153:BM153)</f>
-        <v>0</v>
+        <v>50265</v>
       </c>
       <c r="E153" s="229"/>
       <c r="F153" s="13">
         <f>$C144*(1+F$7)*F144+$C145*(1+F$7)*F145+$C146*(1+F$7)*F146+$C147*(1+F$7)*F147+$C148*(1+F$7)*F148+$C149*(1+F$7)*F149+$C150*(1+F$7)*F150+$C151*(1+F$7)*F151+$C152*(1+F$7)*F152</f>
-        <v>0</v>
+        <v>30744</v>
       </c>
       <c r="G153" s="13">
         <f>$C144*(1+G$7)*G144+$C145*(1+G$7)*G145+$C146*(1+G$7)*G146+$C147*(1+G$7)*G147+$C148*(1+G$7)*G148+$C149*(1+G$7)*G149+$C150*(1+G$7)*G150+$C151*(1+G$7)*G151+$C152*(1+G$7)*G152</f>
-        <v>0</v>
+        <v>8235</v>
       </c>
       <c r="H153" s="13">
         <f t="shared" ref="H153:BL153" si="84">$C144*(1+H$7)*H144+$C145*(1+H$7)*H145+$C146*(1+H$7)*H146+$C147*(1+H$7)*H147+$C148*(1+H$7)*H148+$C149*(1+H$7)*H149+$C150*(1+H$7)*H150+$C151*(1+H$7)*H151+$C152*(1+H$7)*H152</f>
-        <v>0</v>
+        <v>11286</v>
       </c>
       <c r="I153" s="13">
         <f t="shared" si="84"/>
@@ -29449,20 +29487,20 @@
       </c>
       <c r="D154" s="184">
         <f>SUM(F154:BM154)</f>
-        <v>0</v>
+        <v>90477.000000000015</v>
       </c>
       <c r="E154" s="229"/>
       <c r="F154" s="13">
         <f>$C154*F153</f>
-        <v>0</v>
+        <v>55339.200000000004</v>
       </c>
       <c r="G154" s="13">
         <f t="shared" ref="G154:BM154" si="85">$C154*G153</f>
-        <v>0</v>
+        <v>14823</v>
       </c>
       <c r="H154" s="13">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>20314.8</v>
       </c>
       <c r="I154" s="13">
         <f t="shared" si="85"/>
@@ -29955,23 +29993,23 @@
       <c r="C156" s="90"/>
       <c r="D156" s="184">
         <f>SUM(F156:BM156)</f>
-        <v>0</v>
+        <v>140742</v>
       </c>
       <c r="E156" s="230">
         <f>+E146+E147+E150</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F156" s="81">
         <f>F153+F154+F155</f>
-        <v>0</v>
+        <v>86083.200000000012</v>
       </c>
       <c r="G156" s="81">
         <f>G153+G154+G155</f>
-        <v>0</v>
+        <v>23058</v>
       </c>
       <c r="H156" s="81">
         <f t="shared" ref="H156:BM156" si="87">H153+H154+H155</f>
-        <v>0</v>
+        <v>31600.799999999999</v>
       </c>
       <c r="I156" s="81">
         <f t="shared" si="87"/>
@@ -30475,9 +30513,11 @@
       <c r="D159" s="201"/>
       <c r="E159" s="203">
         <f>SUM(F159:BM159)</f>
-        <v>0</v>
-      </c>
-      <c r="F159" s="203"/>
+        <v>10</v>
+      </c>
+      <c r="F159" s="203">
+        <v>10</v>
+      </c>
       <c r="G159" s="203"/>
       <c r="H159" s="203"/>
       <c r="I159" s="203"/>
@@ -30549,9 +30589,11 @@
       <c r="D160" s="202"/>
       <c r="E160" s="203">
         <f t="shared" ref="E160:E167" si="88">SUM(F160:BM160)</f>
-        <v>0</v>
-      </c>
-      <c r="F160" s="203"/>
+        <v>10</v>
+      </c>
+      <c r="F160" s="203">
+        <v>10</v>
+      </c>
       <c r="G160" s="203"/>
       <c r="H160" s="203"/>
       <c r="I160" s="203"/>
@@ -30771,13 +30813,17 @@
       <c r="D163" s="202"/>
       <c r="E163" s="203">
         <f t="shared" si="88"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F163" s="203"/>
-      <c r="G163" s="203"/>
+      <c r="G163" s="203">
+        <v>10</v>
+      </c>
       <c r="H163" s="203"/>
       <c r="I163" s="203"/>
-      <c r="J163" s="203"/>
+      <c r="J163" s="203">
+        <v>10</v>
+      </c>
       <c r="K163" s="203"/>
       <c r="L163" s="203"/>
       <c r="M163" s="203"/>
@@ -31067,9 +31113,11 @@
       <c r="D167" s="201"/>
       <c r="E167" s="203">
         <f t="shared" si="88"/>
-        <v>0</v>
-      </c>
-      <c r="F167" s="203"/>
+        <v>10</v>
+      </c>
+      <c r="F167" s="203">
+        <v>10</v>
+      </c>
       <c r="G167" s="203"/>
       <c r="H167" s="203"/>
       <c r="I167" s="203"/>
@@ -31138,16 +31186,16 @@
       <c r="C168" s="17"/>
       <c r="D168" s="184">
         <f>SUM(F168:BM168)</f>
-        <v>0</v>
+        <v>28590</v>
       </c>
       <c r="E168" s="229"/>
       <c r="F168" s="13">
         <f>$C159*(1+F$7)*F159+$C160*(1+F$7)*F160+$C161*(1+F$7)*F161+$C162*(1+F$7)*F162+$C163*(1+F$7)*F163+$C164*(1+F$7)*F164+$C165*(1+F$7)*F165+$C166*(1+F$7)*F166+$C167*(1+F$7)*F167</f>
-        <v>0</v>
+        <v>20110</v>
       </c>
       <c r="G168" s="13">
         <f>$C159*(1+G$7)*G159+$C160*(1+G$7)*G160+$C161*(1+G$7)*G161+$C162*(1+G$7)*G162+$C163*(1+G$7)*G163+$C164*(1+G$7)*G164+$C165*(1+G$7)*G165+$C166*(1+G$7)*G166+$C167*(1+G$7)*G167</f>
-        <v>0</v>
+        <v>4240</v>
       </c>
       <c r="H168" s="13">
         <f t="shared" ref="H168:BL168" si="89">$C159*(1+H$7)*H159+$C160*(1+H$7)*H160+$C161*(1+H$7)*H161+$C162*(1+H$7)*H162+$C163*(1+H$7)*H163+$C164*(1+H$7)*H164+$C165*(1+H$7)*H165+$C166*(1+H$7)*H166+$C167*(1+H$7)*H167</f>
@@ -31159,7 +31207,7 @@
       </c>
       <c r="J168" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>4240</v>
       </c>
       <c r="K168" s="13">
         <f t="shared" si="89"/>
@@ -31392,16 +31440,16 @@
       </c>
       <c r="D169" s="184">
         <f>SUM(F169:BM169)</f>
-        <v>0</v>
+        <v>51462</v>
       </c>
       <c r="E169" s="229"/>
       <c r="F169" s="13">
         <f>$C169*F168</f>
-        <v>0</v>
+        <v>36198</v>
       </c>
       <c r="G169" s="13">
         <f t="shared" ref="G169:BM169" si="90">$C169*G168</f>
-        <v>0</v>
+        <v>7632</v>
       </c>
       <c r="H169" s="13">
         <f t="shared" si="90"/>
@@ -31413,7 +31461,7 @@
       </c>
       <c r="J169" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>7632</v>
       </c>
       <c r="K169" s="13">
         <f t="shared" si="90"/>
@@ -31898,7 +31946,7 @@
       <c r="C171" s="90"/>
       <c r="D171" s="184">
         <f>SUM(F171:BM171)</f>
-        <v>0</v>
+        <v>80052</v>
       </c>
       <c r="E171" s="230">
         <f>+E161+E162+E165</f>
@@ -31906,11 +31954,11 @@
       </c>
       <c r="F171" s="81">
         <f>F168+F169+F170</f>
-        <v>0</v>
+        <v>56308</v>
       </c>
       <c r="G171" s="81">
         <f>G168+G169+G170</f>
-        <v>0</v>
+        <v>11872</v>
       </c>
       <c r="H171" s="81">
         <f t="shared" ref="H171:BM171" si="92">H168+H169+H170</f>
@@ -31922,7 +31970,7 @@
       </c>
       <c r="J171" s="81">
         <f t="shared" si="92"/>
-        <v>0</v>
+        <v>11872</v>
       </c>
       <c r="K171" s="81">
         <f t="shared" si="92"/>
@@ -32418,9 +32466,11 @@
       <c r="D174" s="201"/>
       <c r="E174" s="203">
         <f>SUM(F174:BM174)</f>
-        <v>0</v>
-      </c>
-      <c r="F174" s="203"/>
+        <v>11</v>
+      </c>
+      <c r="F174" s="203">
+        <v>11</v>
+      </c>
       <c r="G174" s="203"/>
       <c r="H174" s="203"/>
       <c r="I174" s="203"/>
@@ -32566,9 +32616,11 @@
       <c r="D176" s="201"/>
       <c r="E176" s="203">
         <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="F176" s="203"/>
+        <v>11</v>
+      </c>
+      <c r="F176" s="203">
+        <v>11</v>
+      </c>
       <c r="G176" s="203"/>
       <c r="H176" s="203"/>
       <c r="I176" s="203"/>
@@ -32714,11 +32766,13 @@
       <c r="D178" s="202"/>
       <c r="E178" s="203">
         <f t="shared" si="93"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F178" s="203"/>
       <c r="G178" s="203"/>
-      <c r="H178" s="203"/>
+      <c r="H178" s="203">
+        <v>11</v>
+      </c>
       <c r="I178" s="203"/>
       <c r="J178" s="203"/>
       <c r="K178" s="203"/>
@@ -32788,13 +32842,17 @@
       <c r="D179" s="201"/>
       <c r="E179" s="203">
         <f t="shared" si="93"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F179" s="203"/>
-      <c r="G179" s="203"/>
+      <c r="G179" s="203">
+        <v>11</v>
+      </c>
       <c r="H179" s="203"/>
       <c r="I179" s="203"/>
-      <c r="J179" s="203"/>
+      <c r="J179" s="203">
+        <v>11</v>
+      </c>
       <c r="K179" s="203"/>
       <c r="L179" s="203"/>
       <c r="M179" s="203"/>
@@ -33010,9 +33068,11 @@
       <c r="D182" s="201"/>
       <c r="E182" s="203">
         <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="F182" s="203"/>
+        <v>11</v>
+      </c>
+      <c r="F182" s="203">
+        <v>11</v>
+      </c>
       <c r="G182" s="203"/>
       <c r="H182" s="203"/>
       <c r="I182" s="203"/>
@@ -33081,20 +33141,20 @@
       <c r="C183" s="17"/>
       <c r="D183" s="184">
         <f>SUM(F183:BM183)</f>
-        <v>0</v>
+        <v>40128</v>
       </c>
       <c r="E183" s="229"/>
       <c r="F183" s="13">
         <f>$C174*(1+F$7)*F174+$C175*(1+F$7)*F175+$C176*(1+F$7)*F176+$C177*(1+F$7)*F177+$C178*(1+F$7)*F178+$C179*(1+F$7)*F179+$C180*(1+F$7)*F180+$C181*(1+F$7)*F181+$C182*(1+F$7)*F182</f>
-        <v>0</v>
+        <v>22836</v>
       </c>
       <c r="G183" s="13">
         <f>$C174*(1+G$7)*G174+$C175*(1+G$7)*G175+$C176*(1+G$7)*G176+$C177*(1+G$7)*G177+$C178*(1+G$7)*G178+$C179*(1+G$7)*G179+$C180*(1+G$7)*G180+$C181*(1+G$7)*G181+$C182*(1+G$7)*G182</f>
-        <v>0</v>
+        <v>6314</v>
       </c>
       <c r="H183" s="13">
         <f t="shared" ref="H183:BL183" si="94">$C174*(1+H$7)*H174+$C175*(1+H$7)*H175+$C176*(1+H$7)*H176+$C177*(1+H$7)*H177+$C178*(1+H$7)*H178+$C179*(1+H$7)*H179+$C180*(1+H$7)*H180+$C181*(1+H$7)*H181+$C182*(1+H$7)*H182</f>
-        <v>0</v>
+        <v>4664</v>
       </c>
       <c r="I183" s="13">
         <f t="shared" si="94"/>
@@ -33102,7 +33162,7 @@
       </c>
       <c r="J183" s="13">
         <f t="shared" si="94"/>
-        <v>0</v>
+        <v>6314</v>
       </c>
       <c r="K183" s="13">
         <f t="shared" si="94"/>
@@ -33335,20 +33395,20 @@
       </c>
       <c r="D184" s="184">
         <f>SUM(F184:BM184)</f>
-        <v>0</v>
+        <v>72230.399999999994</v>
       </c>
       <c r="E184" s="229"/>
       <c r="F184" s="13">
         <f>$C184*F183</f>
-        <v>0</v>
+        <v>41104.800000000003</v>
       </c>
       <c r="G184" s="13">
         <f t="shared" ref="G184:BM184" si="95">$C184*G183</f>
-        <v>0</v>
+        <v>11365.2</v>
       </c>
       <c r="H184" s="13">
         <f t="shared" si="95"/>
-        <v>0</v>
+        <v>8395.2000000000007</v>
       </c>
       <c r="I184" s="13">
         <f t="shared" si="95"/>
@@ -33356,7 +33416,7 @@
       </c>
       <c r="J184" s="13">
         <f t="shared" si="95"/>
-        <v>0</v>
+        <v>11365.2</v>
       </c>
       <c r="K184" s="13">
         <f t="shared" si="95"/>
@@ -33841,23 +33901,23 @@
       <c r="C186" s="90"/>
       <c r="D186" s="184">
         <f>SUM(F186:BM186)</f>
-        <v>0</v>
+        <v>112358.39999999999</v>
       </c>
       <c r="E186" s="230">
         <f>+E176+E177+E180</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F186" s="81">
         <f>F183+F184+F185</f>
-        <v>0</v>
+        <v>63940.800000000003</v>
       </c>
       <c r="G186" s="81">
         <f>G183+G184+G185</f>
-        <v>0</v>
+        <v>17679.2</v>
       </c>
       <c r="H186" s="81">
         <f t="shared" ref="H186:BM186" si="97">H183+H184+H185</f>
-        <v>0</v>
+        <v>13059.2</v>
       </c>
       <c r="I186" s="81">
         <f t="shared" si="97"/>
@@ -33865,7 +33925,7 @@
       </c>
       <c r="J186" s="81">
         <f t="shared" si="97"/>
-        <v>0</v>
+        <v>17679.2</v>
       </c>
       <c r="K186" s="81">
         <f t="shared" si="97"/>
@@ -34097,20 +34157,20 @@
       <c r="C188" s="249"/>
       <c r="D188" s="218">
         <f>D123+D138+D153+D168+D183</f>
-        <v>0</v>
+        <v>180599</v>
       </c>
       <c r="E188" s="230"/>
       <c r="F188" s="250">
         <f>F123+F138+F153+F168+F183</f>
-        <v>0</v>
+        <v>103206</v>
       </c>
       <c r="G188" s="250">
         <f t="shared" ref="G188:BM190" si="98">G123+G138+G153+G168+G183</f>
-        <v>0</v>
+        <v>28335</v>
       </c>
       <c r="H188" s="250">
         <f t="shared" si="98"/>
-        <v>0</v>
+        <v>38504</v>
       </c>
       <c r="I188" s="250">
         <f t="shared" si="98"/>
@@ -34118,7 +34178,7 @@
       </c>
       <c r="J188" s="250">
         <f t="shared" si="98"/>
-        <v>0</v>
+        <v>10554</v>
       </c>
       <c r="K188" s="250">
         <f t="shared" si="98"/>
@@ -34347,20 +34407,20 @@
       <c r="C189" s="249"/>
       <c r="D189" s="218">
         <f>D124+D139+D154+D169+D184</f>
-        <v>0</v>
+        <v>325078.19999999995</v>
       </c>
       <c r="E189" s="230"/>
       <c r="F189" s="250">
         <f t="shared" ref="F189:U190" si="99">F124+F139+F154+F169+F184</f>
-        <v>0</v>
+        <v>185770.8</v>
       </c>
       <c r="G189" s="250">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>51003</v>
       </c>
       <c r="H189" s="250">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>69307.199999999997</v>
       </c>
       <c r="I189" s="250">
         <f t="shared" si="99"/>
@@ -34368,7 +34428,7 @@
       </c>
       <c r="J189" s="250">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>18997.2</v>
       </c>
       <c r="K189" s="250">
         <f t="shared" si="99"/>
@@ -35053,9 +35113,11 @@
       <c r="D193" s="89"/>
       <c r="E193" s="227">
         <f>SUM(F193:BM193)</f>
-        <v>0</v>
-      </c>
-      <c r="F193" s="70"/>
+        <v>12</v>
+      </c>
+      <c r="F193" s="70">
+        <v>12</v>
+      </c>
       <c r="G193" s="70"/>
       <c r="H193" s="70"/>
       <c r="I193" s="70"/>
@@ -35349,11 +35411,15 @@
       <c r="D197" s="89"/>
       <c r="E197" s="227">
         <f t="shared" si="101"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F197" s="70"/>
-      <c r="G197" s="70"/>
-      <c r="H197" s="70"/>
+      <c r="G197" s="70">
+        <v>12</v>
+      </c>
+      <c r="H197" s="70">
+        <v>12</v>
+      </c>
       <c r="I197" s="70"/>
       <c r="J197" s="70"/>
       <c r="K197" s="70"/>
@@ -35423,9 +35489,11 @@
       <c r="D198" s="89"/>
       <c r="E198" s="227">
         <f t="shared" si="101"/>
-        <v>0</v>
-      </c>
-      <c r="F198" s="70"/>
+        <v>12</v>
+      </c>
+      <c r="F198" s="70">
+        <v>12</v>
+      </c>
       <c r="G198" s="70"/>
       <c r="H198" s="70"/>
       <c r="I198" s="70"/>
@@ -35645,11 +35713,15 @@
       <c r="D201" s="4"/>
       <c r="E201" s="227">
         <f t="shared" si="101"/>
-        <v>0</v>
-      </c>
-      <c r="F201" s="70"/>
+        <v>24</v>
+      </c>
+      <c r="F201" s="70">
+        <v>12</v>
+      </c>
       <c r="G201" s="70"/>
-      <c r="H201" s="70"/>
+      <c r="H201" s="70">
+        <v>12</v>
+      </c>
       <c r="I201" s="70"/>
       <c r="J201" s="70"/>
       <c r="K201" s="70"/>
@@ -35716,20 +35788,20 @@
       <c r="C202" s="17"/>
       <c r="D202" s="184">
         <f>SUM(F202:BM202)</f>
-        <v>0</v>
+        <v>59856</v>
       </c>
       <c r="E202" s="229"/>
       <c r="F202" s="13">
         <f>$C193*(1+F$7)*F193+$C194*(1+F$7)*F194+$C195*(1+F$7)*F195+$C196*(1+F$7)*F196+$C197*(1+F$7)*F197+$C198*(1+F$7)*F198+$C199*(1+F$7)*F199+$C200*(1+F$7)*F200+$C201*(1+F$7)*F201</f>
-        <v>0</v>
+        <v>29016</v>
       </c>
       <c r="G202" s="13">
         <f t="shared" ref="G202:BL202" si="102">$C193*(1+G$7)*G193+$C194*(1+G$7)*G194+$C195*(1+G$7)*G195+$C196*(1+G$7)*G196+$C197*(1+G$7)*G197+$C198*(1+G$7)*G198+$C199*(1+G$7)*G199+$C200*(1+G$7)*G200+$C201*(1+G$7)*G201</f>
-        <v>0</v>
+        <v>5088</v>
       </c>
       <c r="H202" s="13">
         <f t="shared" si="102"/>
-        <v>0</v>
+        <v>25752</v>
       </c>
       <c r="I202" s="13">
         <f t="shared" si="102"/>
@@ -35970,20 +36042,20 @@
       </c>
       <c r="D203" s="184">
         <f>SUM(F203:BM203)</f>
-        <v>0</v>
+        <v>107740.8</v>
       </c>
       <c r="E203" s="229"/>
       <c r="F203" s="13">
         <f>$C203*F202</f>
-        <v>0</v>
+        <v>52228.800000000003</v>
       </c>
       <c r="G203" s="13">
         <f t="shared" ref="G203:BM203" si="103">$C203*G202</f>
-        <v>0</v>
+        <v>9158.4</v>
       </c>
       <c r="H203" s="13">
         <f t="shared" si="103"/>
-        <v>0</v>
+        <v>46353.599999999999</v>
       </c>
       <c r="I203" s="13">
         <f t="shared" si="103"/>
@@ -36476,20 +36548,20 @@
       <c r="C205" s="90"/>
       <c r="D205" s="184">
         <f>SUM(F205:BM205)</f>
-        <v>0</v>
+        <v>167596.79999999999</v>
       </c>
       <c r="E205" s="230"/>
       <c r="F205" s="81">
         <f>F202+F203+F204</f>
-        <v>0</v>
+        <v>81244.800000000003</v>
       </c>
       <c r="G205" s="81">
         <f>G202+G203+G204</f>
-        <v>0</v>
+        <v>14246.4</v>
       </c>
       <c r="H205" s="81">
         <f t="shared" ref="H205:BM205" si="105">H202+H203+H204</f>
-        <v>0</v>
+        <v>72105.600000000006</v>
       </c>
       <c r="I205" s="81">
         <f t="shared" si="105"/>
@@ -36927,11 +36999,15 @@
       <c r="D209" s="209"/>
       <c r="E209" s="227">
         <f>SUM(F209:BM209)</f>
-        <v>0</v>
-      </c>
-      <c r="F209" s="203"/>
+        <v>26</v>
+      </c>
+      <c r="F209" s="203">
+        <v>13</v>
+      </c>
       <c r="G209" s="203"/>
-      <c r="H209" s="203"/>
+      <c r="H209" s="203">
+        <v>13</v>
+      </c>
       <c r="I209" s="203"/>
       <c r="J209" s="203"/>
       <c r="K209" s="203"/>
@@ -37143,11 +37219,15 @@
       <c r="D212" s="209"/>
       <c r="E212" s="227">
         <f t="shared" si="106"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F212" s="203"/>
-      <c r="G212" s="203"/>
-      <c r="H212" s="203"/>
+      <c r="G212" s="203">
+        <v>13</v>
+      </c>
+      <c r="H212" s="203">
+        <v>13</v>
+      </c>
       <c r="I212" s="203"/>
       <c r="J212" s="203"/>
       <c r="K212" s="203"/>
@@ -37215,9 +37295,11 @@
       <c r="D213" s="209"/>
       <c r="E213" s="227">
         <f t="shared" si="106"/>
-        <v>0</v>
-      </c>
-      <c r="F213" s="203"/>
+        <v>13</v>
+      </c>
+      <c r="F213" s="203">
+        <v>13</v>
+      </c>
       <c r="G213" s="203"/>
       <c r="H213" s="203"/>
       <c r="I213" s="203"/>
@@ -37503,9 +37585,11 @@
       <c r="D217" s="201"/>
       <c r="E217" s="227">
         <f t="shared" si="106"/>
-        <v>0</v>
-      </c>
-      <c r="F217" s="203"/>
+        <v>13</v>
+      </c>
+      <c r="F217" s="203">
+        <v>13</v>
+      </c>
       <c r="G217" s="203"/>
       <c r="H217" s="203"/>
       <c r="I217" s="203"/>
@@ -38586,20 +38670,20 @@
       <c r="C222" s="316"/>
       <c r="D222" s="184">
         <f>D93+D108+D188+D202+D218</f>
-        <v>1037484.3200000001</v>
+        <v>1298435.32</v>
       </c>
       <c r="E222" s="229"/>
       <c r="F222" s="184">
         <f t="shared" ref="F222:AK222" si="111">F93+F108+F188+F202+F218</f>
-        <v>85920</v>
+        <v>238638</v>
       </c>
       <c r="G222" s="184">
         <f t="shared" si="111"/>
-        <v>85920</v>
+        <v>119343</v>
       </c>
       <c r="H222" s="184">
         <f t="shared" si="111"/>
-        <v>85920</v>
+        <v>150176</v>
       </c>
       <c r="I222" s="184">
         <f t="shared" si="111"/>
@@ -38607,7 +38691,7 @@
       </c>
       <c r="J222" s="184">
         <f t="shared" si="111"/>
-        <v>85920</v>
+        <v>96474</v>
       </c>
       <c r="K222" s="184">
         <f t="shared" si="111"/>
@@ -38838,20 +38922,20 @@
       <c r="C223" s="304"/>
       <c r="D223" s="184">
         <f>D94+D109+D189+D203+D219</f>
-        <v>1867471.7759999998</v>
+        <v>2337183.5759999994</v>
       </c>
       <c r="E223" s="229"/>
       <c r="F223" s="184">
         <f t="shared" ref="F223:AK223" si="113">F94+F109+F189+F203+F219</f>
-        <v>154656</v>
+        <v>429548.39999999997</v>
       </c>
       <c r="G223" s="184">
         <f t="shared" si="113"/>
-        <v>154656</v>
+        <v>214817.4</v>
       </c>
       <c r="H223" s="184">
         <f t="shared" si="113"/>
-        <v>154656</v>
+        <v>270316.79999999999</v>
       </c>
       <c r="I223" s="184">
         <f t="shared" si="113"/>
@@ -38859,7 +38943,7 @@
       </c>
       <c r="J223" s="184">
         <f t="shared" si="113"/>
-        <v>154656</v>
+        <v>173653.2</v>
       </c>
       <c r="K223" s="184">
         <f t="shared" si="113"/>
@@ -39342,20 +39426,20 @@
       <c r="C225" s="307"/>
       <c r="D225" s="184">
         <f>D96+D111+D191+D205+D221</f>
-        <v>2904956.0960000004</v>
+        <v>3129941.696</v>
       </c>
       <c r="E225" s="229"/>
       <c r="F225" s="184">
         <f t="shared" ref="F225:AK225" si="117">F96+F111+F191+F205+F221</f>
-        <v>240575.99999999997</v>
+        <v>379209.6</v>
       </c>
       <c r="G225" s="184">
         <f t="shared" si="117"/>
-        <v>240575.99999999997</v>
+        <v>254822.39999999997</v>
       </c>
       <c r="H225" s="184">
         <f t="shared" si="117"/>
-        <v>240575.99999999997</v>
+        <v>312681.59999999998</v>
       </c>
       <c r="I225" s="184">
         <f t="shared" si="117"/>
@@ -44896,7 +44980,7 @@
     <row r="61" spans="1:66" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D61" s="242">
         <f>SUM(F64:BM64)</f>
-        <v>-525204.81381333328</v>
+        <v>-669431.96448000032</v>
       </c>
       <c r="E61" s="243" t="s">
         <v>195</v>
@@ -44905,486 +44989,486 @@
     <row r="63" spans="1:66" hidden="1" x14ac:dyDescent="0.2">
       <c r="F63" s="190">
         <f>Forecast!E28*Expenses!$D$60/12</f>
-        <v>-939.06333333333339</v>
+        <v>-2364.431333333333</v>
       </c>
       <c r="G63" s="190">
         <f>Forecast!F28*Expenses!$D$60/12</f>
-        <v>-1740.9833333333333</v>
+        <v>-3478.2993333333329</v>
       </c>
       <c r="H63" s="190">
         <f>Forecast!G28*Expenses!$D$60/12</f>
-        <v>-2542.9033333333332</v>
+        <v>-4879.942</v>
       </c>
       <c r="I63" s="190">
         <f>Forecast!H28*Expenses!$D$60/12</f>
-        <v>-3344.8233333333333</v>
+        <v>-5681.8620000000001</v>
       </c>
       <c r="J63" s="190">
         <f>Forecast!I28*Expenses!$D$60/12</f>
-        <v>-4146.7433333333329</v>
+        <v>-6582.2860000000001</v>
       </c>
       <c r="K63" s="190">
         <f>Forecast!J28*Expenses!$D$60/12</f>
-        <v>-4948.663333333333</v>
+        <v>-7384.2059999999992</v>
       </c>
       <c r="L63" s="190">
         <f>Forecast!K28*Expenses!$D$60/12</f>
-        <v>-5750.583333333333</v>
+        <v>-8186.1259999999993</v>
       </c>
       <c r="M63" s="190">
         <f>Forecast!L28*Expenses!$D$60/12</f>
-        <v>-6511.170000000001</v>
+        <v>-8946.7126666666663</v>
       </c>
       <c r="N63" s="190">
         <f>Forecast!M28*Expenses!$D$60/12</f>
-        <v>-7313.09</v>
+        <v>-9748.6326666666664</v>
       </c>
       <c r="O63" s="190">
         <f>Forecast!N28*Expenses!$D$60/12</f>
-        <v>-7979.0766666666668</v>
+        <v>-10414.619333333334</v>
       </c>
       <c r="P63" s="190">
         <f>Forecast!O28*Expenses!$D$60/12</f>
-        <v>-8780.9966666666678</v>
+        <v>-11216.539333333334</v>
       </c>
       <c r="Q63" s="190">
         <f>Forecast!P28*Expenses!$D$60/12</f>
-        <v>-9534.4500000000007</v>
+        <v>-11969.992666666665</v>
       </c>
       <c r="R63" s="190">
         <f>Forecast!Q28*Expenses!$D$60/12</f>
-        <v>-9534.4500000000007</v>
+        <v>-11969.992666666665</v>
       </c>
       <c r="S63" s="190">
         <f>Forecast!R28*Expenses!$D$60/12</f>
-        <v>-9547.2477400000007</v>
+        <v>-11982.790406666667</v>
       </c>
       <c r="T63" s="190">
         <f>Forecast!S28*Expenses!$D$60/12</f>
-        <v>-9547.2477400000007</v>
+        <v>-11982.790406666667</v>
       </c>
       <c r="U63" s="190">
         <f>Forecast!T28*Expenses!$D$60/12</f>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="V63" s="190">
         <f>Forecast!U28*Expenses!$D$60/12</f>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="W63" s="190">
         <f>Forecast!V28*Expenses!$D$60/12</f>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="X63" s="190">
         <f>Forecast!W28*Expenses!$D$60/12</f>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="Y63" s="190">
         <f>Forecast!X28*Expenses!$D$60/12</f>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="Z63" s="190">
         <f>Forecast!Y28*Expenses!$D$60/12</f>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="AA63" s="190">
         <f>Forecast!Z28*Expenses!$D$60/12</f>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AB63" s="190">
         <f>Forecast!AA28*Expenses!$D$60/12</f>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AC63" s="190">
         <f>Forecast!AB28*Expenses!$D$60/12</f>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AD63" s="190">
         <f>Forecast!AC28*Expenses!$D$60/12</f>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AE63" s="190">
         <f>Forecast!AD28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AF63" s="190">
         <f>Forecast!AE28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AG63" s="190">
         <f>Forecast!AF28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AH63" s="190">
         <f>Forecast!AG28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AI63" s="190">
         <f>Forecast!AH28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AJ63" s="190">
         <f>Forecast!AI28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AK63" s="190">
         <f>Forecast!AJ28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AL63" s="190">
         <f>Forecast!AK28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AM63" s="190">
         <f>Forecast!AL28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AN63" s="190">
         <f>Forecast!AM28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AO63" s="190">
         <f>Forecast!AN28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AP63" s="190">
         <f>Forecast!AO28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AQ63" s="190">
         <f>Forecast!AP28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AR63" s="190">
         <f>Forecast!AQ28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AS63" s="190">
         <f>Forecast!AR28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AT63" s="190">
         <f>Forecast!AS28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AU63" s="190">
         <f>Forecast!AT28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AV63" s="190">
         <f>Forecast!AU28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AW63" s="190">
         <f>Forecast!AV28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AX63" s="190">
         <f>Forecast!AW28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AY63" s="190">
         <f>Forecast!AX28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AZ63" s="190">
         <f>Forecast!AY28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BA63" s="190">
         <f>Forecast!AZ28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BB63" s="190">
         <f>Forecast!BA28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BC63" s="190">
         <f>Forecast!BB28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BD63" s="190">
         <f>Forecast!BC28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BE63" s="190">
         <f>Forecast!BD28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BF63" s="190">
         <f>Forecast!BE28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BG63" s="190">
         <f>Forecast!BF28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BH63" s="190">
         <f>Forecast!BG28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BI63" s="190">
         <f>Forecast!BH28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BJ63" s="190">
         <f>Forecast!BI28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BK63" s="190">
         <f>Forecast!BJ28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BL63" s="190">
         <f>Forecast!BK28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BM63" s="190">
         <f>Forecast!BL28*Expenses!$D$60/12</f>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BN63" s="206"/>
     </row>
     <row r="64" spans="1:66" hidden="1" x14ac:dyDescent="0.2">
       <c r="F64">
         <f>IF(F63&lt;0,F63,0)</f>
-        <v>-939.06333333333339</v>
+        <v>-2364.431333333333</v>
       </c>
       <c r="G64" s="206">
         <f t="shared" ref="G64:BM64" si="8">IF(G63&lt;0,G63,0)</f>
-        <v>-1740.9833333333333</v>
+        <v>-3478.2993333333329</v>
       </c>
       <c r="H64" s="206">
         <f t="shared" si="8"/>
-        <v>-2542.9033333333332</v>
+        <v>-4879.942</v>
       </c>
       <c r="I64" s="206">
         <f t="shared" si="8"/>
-        <v>-3344.8233333333333</v>
+        <v>-5681.8620000000001</v>
       </c>
       <c r="J64" s="206">
         <f t="shared" si="8"/>
-        <v>-4146.7433333333329</v>
+        <v>-6582.2860000000001</v>
       </c>
       <c r="K64" s="206">
         <f t="shared" si="8"/>
-        <v>-4948.663333333333</v>
+        <v>-7384.2059999999992</v>
       </c>
       <c r="L64" s="206">
         <f t="shared" si="8"/>
-        <v>-5750.583333333333</v>
+        <v>-8186.1259999999993</v>
       </c>
       <c r="M64" s="206">
         <f t="shared" si="8"/>
-        <v>-6511.170000000001</v>
+        <v>-8946.7126666666663</v>
       </c>
       <c r="N64" s="206">
         <f t="shared" si="8"/>
-        <v>-7313.09</v>
+        <v>-9748.6326666666664</v>
       </c>
       <c r="O64" s="206">
         <f t="shared" si="8"/>
-        <v>-7979.0766666666668</v>
+        <v>-10414.619333333334</v>
       </c>
       <c r="P64" s="206">
         <f t="shared" si="8"/>
-        <v>-8780.9966666666678</v>
+        <v>-11216.539333333334</v>
       </c>
       <c r="Q64" s="206">
         <f t="shared" si="8"/>
-        <v>-9534.4500000000007</v>
+        <v>-11969.992666666665</v>
       </c>
       <c r="R64" s="206">
         <f t="shared" si="8"/>
-        <v>-9534.4500000000007</v>
+        <v>-11969.992666666665</v>
       </c>
       <c r="S64" s="206">
         <f t="shared" si="8"/>
-        <v>-9547.2477400000007</v>
+        <v>-11982.790406666667</v>
       </c>
       <c r="T64" s="206">
         <f t="shared" si="8"/>
-        <v>-9547.2477400000007</v>
+        <v>-11982.790406666667</v>
       </c>
       <c r="U64" s="206">
         <f t="shared" si="8"/>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="V64" s="206">
         <f t="shared" si="8"/>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="W64" s="206">
         <f t="shared" si="8"/>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="X64" s="206">
         <f t="shared" si="8"/>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="Y64" s="206">
         <f t="shared" si="8"/>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="Z64" s="206">
         <f t="shared" si="8"/>
-        <v>-9608.1260466666681</v>
+        <v>-12043.668713333334</v>
       </c>
       <c r="AA64" s="206">
         <f t="shared" si="8"/>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AB64" s="206">
         <f t="shared" si="8"/>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AC64" s="206">
         <f t="shared" si="8"/>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AD64" s="206">
         <f t="shared" si="8"/>
-        <v>-9598.1260466666681</v>
+        <v>-12033.668713333334</v>
       </c>
       <c r="AE64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AF64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AG64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AH64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AI64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AJ64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AK64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AL64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AM64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AN64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AO64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AP64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AQ64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AR64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AS64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AT64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AU64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AV64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AW64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AX64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AY64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="AZ64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BA64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BB64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BC64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BD64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BE64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BF64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BG64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BH64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BI64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BJ64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BK64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BL64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
       <c r="BM64" s="206">
         <f t="shared" si="8"/>
-        <v>-9628.630320000002</v>
+        <v>-12064.172986666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>